<commit_message>
adding count in Total Column
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -462,6 +462,9 @@
       <c r="J4">
         <v>77</v>
       </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:K9" si="0">=SUM(E4:J4)</f>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -494,6 +497,29 @@
       <c r="J5">
         <v>12</v>
       </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="K6">
+        <f t="shared" si="0"/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="K7">
+        <f t="shared" si="0"/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="K8">
+        <f t="shared" si="0"/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="K9">
+        <f t="shared" si="0"/>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
merge cells: famoso mesclar e centralizar
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -522,5 +522,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+  </mergeCells>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
stylinh cells: color and width
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -85,12 +85,22 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD07462"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DFB9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,8 +115,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,20 +395,23 @@
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="true" max="11" min="4" width="14"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -526,7 +545,7 @@
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H2:K2"/>
   </mergeCells>
 </worksheet>
 </file>
</xml_diff>